<commit_message>
fixing links for excel spreadsheet pages
</commit_message>
<xml_diff>
--- a/Master Costs Workbook Using Sample Data.xlsx
+++ b/Master Costs Workbook Using Sample Data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{B3E2F1D2-E1E9-45D9-BEF3-EAA3AC8E86EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5EE3FF-7C22-40CA-BD4B-BFA090976DC8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{C089D296-1CBC-4FD8-8051-3293806BE7B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C089D296-1CBC-4FD8-8051-3293806BE7B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Appetizer" sheetId="1" r:id="rId1"/>
@@ -4703,7 +4703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52485BFC-EAA8-4A9D-8187-6DDA64CD4038}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7351,13 +7351,13 @@
         <cfvo type="num" val="2"/>
       </iconSet>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="113" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="113" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="114" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="114" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="115" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="115" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8161,13 +8161,13 @@
         <cfvo type="num" val="2"/>
       </iconSet>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9189,13 +9189,13 @@
         <cfvo type="num" val="2"/>
       </iconSet>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9261,7 +9261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58C4586-B628-4825-B784-621367264176}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -10024,13 +10024,13 @@
         <cfvo type="num" val="2"/>
       </iconSet>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Final changes to portfolio
</commit_message>
<xml_diff>
--- a/Master Costs Workbook Using Sample Data.xlsx
+++ b/Master Costs Workbook Using Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/caada7bb5bb16b10/Documents/GitHub/Cieri.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{B3E2F1D2-E1E9-45D9-BEF3-EAA3AC8E86EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5EE3FF-7C22-40CA-BD4B-BFA090976DC8}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6EC8D51F-7F51-4BF8-98CB-1D65034D3E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B855688-B03F-4080-AAD9-1B70A817B5E1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{C089D296-1CBC-4FD8-8051-3293806BE7B9}"/>
+    <workbookView xWindow="-28920" yWindow="-8175" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C089D296-1CBC-4FD8-8051-3293806BE7B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Appetizer" sheetId="1" r:id="rId1"/>
@@ -4703,7 +4703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52485BFC-EAA8-4A9D-8187-6DDA64CD4038}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -6455,8 +6455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95861C51-69AD-4BA5-A769-127DC8992690}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>